<commit_message>
Get daily reddit data: Tue May 28 08:09:49 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_02.xlsx
+++ b/data/2024_06_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C472"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2913 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1d2e6g6</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Pearl chrome almond french tip❤️with a normal pose as a palate cleanser</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iacucm5gj43d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1d2dnya</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone ever have gel polish peeled off with little nail pliers? </t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2dnya/anyone_ever_have_gel_polish_peeled_off_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1d2cymk</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is $50 fair for this? </t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cycg500w343d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1d2cbzp</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails beginner advice please (amab) </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2cbzp/nails_beginner_advice_please_amab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1d2bt8p</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>News nails 🤩</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cassd2v2q33d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1d2bl4p</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Did my daughters nails. My attempt at mushrooms.</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2bl4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1d2beq9</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Broken toenail</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypgty2ill33d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1d2ar4i</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>My nails 💕💕💕</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imkdbnvee33d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1d29tya</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Would It be silly of me to get my nails done even though I chew on them?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d29tya/would_it_be_silly_of_me_to_get_my_nails_done_even/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1d29t1w</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>unintentional buzzball nails</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d29t1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1d29l89</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Prom nails?!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d29l89</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1d29gtz</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Perfect Nude/Pink Color For Asian Tone Skin?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d29gtz/perfect_nudepink_color_for_asian_tone_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1d29fye</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>First time nails</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wbqaun6133d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1d296ub</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Super simple nude nails</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d296ub</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1d296ab</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Ombré chrome</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f77ilvnly23d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1d295ah</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>diy milky white</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d295ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1d291z8</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>There are times I'm a Barbie girl and other times I'm just Wednesday Addams, I can't choose just one style, can you too? 😅</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d291z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1d291w5</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>I’m proud of this set. I’m new to dip so it’s not perfect yet</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d291w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1d28k5s</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Guess the theme</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d28k5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1d28ao7</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>latest set</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvw3kci8q23d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1d28ahl</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best builder gel for beginners? Can you add builder gel on top of tips to strengthen them? </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d28ahl/best_builder_gel_for_beginners_can_you_add/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1d27pqp</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Did my sisters nails and loveee them</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d27pqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1d27jm7</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Learning how to do my own acrylics, absolutely hate this set what can I add to make them bearable (I just spent 2 hours giving myself a fill I don't want to file them and start over </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d27jm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1d2753c</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Chrome w pink French</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2753c</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1d273nz</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>First time doing gel Milky White - French</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9d2v4dve23d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1d271lt</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Chrome nails! I love the look but is powder chrome a losing battle? I’ve tried everything and they chip instantly</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d271lt</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1d26n1t</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>White/pink polish</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr4x4qlka23d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1d26fi0</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>first time doing gel polish😭</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5jdbzmm823d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1d25opo</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>I love these colors 💙💚</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d25opo</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1d25g7p</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombré French dip- started dip 2 months ago and this is the longest my natural nails have ever been. </t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhgj3m75023d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1d258vq</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>What do you think of this technique? Ive already thought of a million combos I wanna do in this style 😅</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d258vq</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1d24hdv</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Thoughts on 2JOY nail polishes?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibel9kfxr13d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1d24fwt</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>best place on etsy to get custom game 3 nails? my nail beds are too wide for the store bought ones!:(</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcbvns7lr13d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1d24ap7</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Oranges anyone ? 🍊</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d24ap7</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1d246jl</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>DIY set</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88idpnsdp13d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1d23t71</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>RK - Frosty Sky Blue (i got this from a weird beauty supply with no products id seen before lol)</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d23t71</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1d23ghp</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>What do we think of these?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhdjojvjj13d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1d23fkt</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Garden party</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d23fkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1d23ehe</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>I never want to take these off!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rd848174j13d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1d23cft</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done today 🦋.  Best set I’ve had for sure !!  </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d23cft</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1d22q0k</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>I love these ⭐️🌛</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gpyoj45rd13d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1d22b49</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Got BIAB yesterday and some are coming away, advice please.</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d22b49</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1d2253u</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9xwqwi8913d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1d21s4f</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Heard we were getting ~*unhinged*~</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d21s4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1d215qg</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Is this combination good? I fell in love💗 💕</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjnghvdq113d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1d210qf</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Help! Dip topcoat issue</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d210qf/help_dip_topcoat_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1d210mw</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Help! Dip topcoat issue</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d210mw/help_dip_topcoat_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1d20u3n</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Before &amp; After 💜</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d20u3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1d20q2d</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Ladybug nail art :)</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d20q2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1d20mma</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Got my nails painted!</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d20mma</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1d20m44</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this shade of pink </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jf8531jcy03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1d20ax2</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Is this normal after getting fake nails removed? This was my first time having them. Any advice on caring for them now?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x86vpspbw03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1d202bv</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>builder gel not curing</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d202bv/builder_gel_not_curing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1d1zpim</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>My nail tech kills it every time 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kovgdyags03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1d1zojr</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Is this peeling normal for acrylic nails? How to avoid?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3agf1ao9s03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1d1zlh5</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Got told yesterday I have pretty hands</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tupemhjpr03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1d1zfn0</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>my first set of press on nailzzz💅🏼</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lij39z6nq03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1d1z67f</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>French ombré gel wedding nails! Haven’t had a gel set in years</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gpmsb2lo03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1d1z1h9</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>I know we love cateye, but do we love aggressively holo cateye?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1z1h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1d1z10c</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are my nails fully cured? </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c89njjpon03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1d1yw44</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>What’s a good file bit for my nail drill that can effectively file down my Gel-x nails?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d1yw44/whats_a_good_file_bit_for_my_nail_drill_that_can/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1d1yu40</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun summer gel x set </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxl9utg8m03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1d1yu0m</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Dashing diva gelxtend clear nails</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzdktjv7m03d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1d1yp61</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>blue chrome</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qphyir27l03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1d1xpza</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite gel manicure of mine </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dku5rfyqd03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1d1xdb0</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>As the darkness takes over</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7om0r221b03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1d1xc7q</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets💅🏻</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1xc7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1d1wv41</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Current nails 💞</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1wv41</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1d1woti</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Has anyone tried glueing nail tips on with builder gel?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d1woti/has_anyone_tried_glueing_nail_tips_on_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1d1w6h1</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>changed my manicurist and i think she did a better job than the last one🥹🩷</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1w6h1</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1d1w22a</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>A couple of different styles I did on myself</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1w22a</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1d1vxph</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>since some didn’t get my previous post was an obvious joke or simply didn’t have a sense of humour here are “normal” pics of my nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1vxph</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1d1vk9i</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Are my thumbs too wide for almond shape?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1vk9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1d1vi20</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>First time testing out nail art!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1vi20</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1d1v8fx</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying the almond shape and I think it suits my hands so well! </t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsa1jz2puz2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1d1upjd</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>I think I made real knives 😨</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1upjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1d1u8fs</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Wedding Naiks</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d1u8fs/wedding_naiks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1d1u82q</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I asked for cute nails and got cute nails 🥰 </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7mels4wmz2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1d1tpfq</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Nude is the new red</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1tpfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1d1tlf0</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>doing everything to keep my gel x on but they still keep popping off! :(</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xswmvgqzhz2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1d1tday</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My friend &amp; I got some chocolates and we both have cute summer nails right now! (Did not know which flair to choose) </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j940vzlagz2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1d1t2zv</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Changed my nails after appointment 💅🫠</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1t2zv</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1d1smwu</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOONCAT - Petals for a narcissist </t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1smwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1d1sm0s</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Bedazzled ✨</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1sm0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1d1sju5</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>I did glittery nails!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b69k97m9z2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1d1sj12</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>The best nails I’ve done so far</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pba5eydf9z2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1d1s45x</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Do you know what this is?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hixmdp636z2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1d1rvwo</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Fresh Set 💅🤘🏼</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1rvwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1d1rg9v</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Strawberry nails🍓</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1rg9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1d1rch2</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>10th attempt at polygels and they’re finally going right!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1rch2</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1d1qqs1</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Bonding with Mum, but my nails end up bleeding</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/19kkqoumty2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1d1qc8z</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Help me take care of my hands pre engagement! I am a licensed Cosmo!!!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d1qc8z/help_me_take_care_of_my_hands_pre_engagement_i_am/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1d1pt94</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>tried my best 🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1pt94</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1d1pnzk</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Are all of you getting acrylics?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d1pnzk/are_all_of_you_getting_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1d1pf9e</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Pearly nail polish 🫧🐚</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2ceolq6gy2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1d1pc3z</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Bollywood pedi</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1pc3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1d1p0a0</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>SOS</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1p0a0</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1d1ox07</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Ribbons and roses 🩷</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1ox07</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1d1ojib</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Where can I find a polish this color?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1ojib</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1d1obba</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Have to keep short nails for the first time in years. What can I do to make them more lively?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9t757wpr2y2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1d2d97r</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Literally my camera roll after trying thermal polish for the first time:</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/noxk8q3k743d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1d2c5t4</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Nail Envy new formula causing nail to lift from the nail bed </t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d2c5t4/opi_nail_envy_new_formula_causing_nail_to_lift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1d2bhe4</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mermaid nails! Hard to catch the actual shift in the light, but I love them! </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glfi2l1im33d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1d2ajd0</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does a “flawless filter” for nails exist? </t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d2ajd0/does_a_flawless_filter_for_nails_exist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1d2adad</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Transitional autumn winter vibes! 🌰✨🥰</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/413npmuha33d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1d2a1re</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Eternal Nail Polishes</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hu0mh76733d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1d29xie</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Taaale as ooold as tiiime 💀😂</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bg3wmccz533d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1d28wt5</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black &amp; Purp 🖤💜 </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d28wt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1d28pld</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>2 years of progress with gel designs!</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d28pld</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1d27xaz</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Top coat causing bubbles?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d27xaz/top_coat_causing_bubbles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1d277dw</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh lime margaritas and Apres Extra Guac 🥑 </t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1jmkiztf23d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1d274o2</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Glittery but not metallic</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d274o2/glittery_but_not_metallic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1d26t66</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Emily de Molly Sale</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.emilydemolly.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1d26iim</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>green or yellow ?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d26iim</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1d25xmj</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>A questionable jelly sandwich experiment</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d25xmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1d25kjl</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Attack of the 50 ft. Storage Cabinet!!</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d25kjl</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1d25j6p</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>How it started versus how it’s going</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d25j6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1d2590o</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Such a pretty glow</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x25cirley13d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1d255qr</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Citron Jelly + Saffron Jelly</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x4ax1blx13d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1d254dn</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>How long does Essie last for y’all?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d254dn/how_long_does_essie_last_for_yall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1d25450</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Can’t wait to take these out!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kt2c7mq7x13d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1d253g7</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Got the whole family involved</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d253g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1d24yhg</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ghost ship magnetic 🧲 </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d24yhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1d244d7</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d244d7</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1d22ujn</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Does anyone else find that their shorties are actually stronger?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d22ujn/does_anyone_else_find_that_their_shorties_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1d22la9</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Dupe for ILNP Flower Child (or Mooncat Moonrise) without the holo</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d22la9/dupe_for_ilnp_flower_child_or_mooncat_moonrise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1d227de</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell, I love it so much!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ktcpv9p913d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1d224cf</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Smiski nails 💚🌟</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d224cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1d21xvm</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Every few weeks I end up with a few broken nails</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yimra5ro713d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1d21m8n</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ISO a nail stamping plate that has spooky eyes. </t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d21m8n/iso_a_nail_stamping_plate_that_has_spooky_eyes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1d215aq</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Is this combination good? I fell in love💗 💕</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6pr80bwk113d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1d20902</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Oldie but man, SUCH a goodie 😍</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d20902</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1d201za</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brands similar to Mooncat </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d201za/brands_similar_to_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1d1zo2y</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Hopped on the hype train</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1zo2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1d1zbej</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Polished for Days — Lush</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1zbej</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1d1yznv</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The most satisfying thing I've ever done!! </t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1yznv</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1d1yu7k</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Am I Everything You Fear x Onism</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1yu7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1d1yfjp</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>My first attempt at interlocking dots nail art</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1yfjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1d1yaeu</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>ILNP Pink Mimosa is so shiny ✨</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1yaeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1d1xs5k</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shimmers, holographics, and sunshine makes me happy. </t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1xs5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1d1xe5f</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time thermal - Leesha's Lacquer </t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1xe5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1d1x4vw</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>One of the prettiest shades I have 🥹</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1x4vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1d1x475</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>I've hopped on the shimmer train, and I couldn't decide.</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1x475</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1d1w9mi</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Giving Mooncat's other thermal some love</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1w9mi</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1d1w3bi</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Pi Colors Cloud Rainbow as compared to an actual moonstone</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1w3bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1d1w3aj</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time in about seven years! </t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc98qtz7103d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1d1w0if</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Orange nails make my heart happy</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqhe50bm003d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1d1vnr3</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Gel X + Mooncat Mercury’s Tears</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1vnr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1d1vd7k</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Picked up House of Hades during the sale</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6crxh1ppvz2d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1d1udgy</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>What do you guys think of men that wear polish?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1udgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1d1t9tc</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Can I please finally get some sun here? 😭</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1t9tc</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1d1t547</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Thick, juicy 3d detailing with top coat!</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hu8qnmziez2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1d1t0dq</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>squishy 🌙 ⭐️</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1t0dq</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1d1sajr</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Question about nail breaks/peeling spots.</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d1sajr/question_about_nail_breakspeeling_spots/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1d1s7cu</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>👀</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1s7cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1d1ri1u</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Have you tried layering jellies? </t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4r6m3tpq0z2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1d1qxek</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Right Way isn't the Only Way </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1qxek</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1d1q1ve</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Blurring base coat?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d1q1ve/blurring_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1d1pev7</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>lol 🫠</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0v2f802gy2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1d1o3vp</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d1o3vp/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1d1nrei</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>This week’s beauties</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1nrei</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1d1nm9r</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Is Marsala Jelly by Cirque Colors normally patchy?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d1nm9r/is_marsala_jelly_by_cirque_colors_normally_patchy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1d2bcas</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>I’m new to this group and wanted to share some of my work💕</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2bcas</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1d1y2o7</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>love to paint mine in total CHAOS</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjzvxpzbg03d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1d1x7zs</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>some of my best sets 💜</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sh9e9vzu903d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1d1wwiv</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>First time doing intricate design on myself</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1wwiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1d1vbhy</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Flag nail art 🇯🇲</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1vbhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1d1urfh</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>What do you think about this my work?  🩶</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1urfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1d1u1l8</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Fire nails to match her hair</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4w090rcilz2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1d1pb8e</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Bollywood</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d1pb8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1d1o1gp</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>i let my boyfriend pick my new nails and i absolutely love them💜✨</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dnjd4cugzx2d1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed May 29 08:09:35 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_02.xlsx
+++ b/data/2024_06_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C472"/>
+  <dimension ref="A1:C644"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8457,6 +8457,2930 @@
         </is>
       </c>
     </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1d36bn5</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When I was 4, a door was slammed onto this finger and broke half of it. It was extremely traumatic, I don't even remember of I am remembering it correctly, but half of the nail is dead? The other half grows just fine. Is this okay? </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1bnggfjhb3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1d35z7c</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>My bday set i madr yesterday c:</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d35z7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1d35hj0</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>nails to go with this dress as a wedding guest?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d35hj0/nails_to_go_with_this_dress_as_a_wedding_guest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1d3472b</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love a good sparkly moment </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qauau84kra3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1d346aq</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>I have an ADHD idea</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d346aq</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1d33bql</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite and last XL set. </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mlubzyu7ia3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1d33a4e</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My most favorite set of nails 💅 </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsdssshrha3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1d336t4</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>2nd time dipping &amp; dotting</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wowg06xga3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1d333sp</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Press On Nails I Wore For My Birthday Last Week</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d333sp</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1d32za5</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>These little beauties have been on a week and a half. Still goin’ strong 💪 💅</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d32za5</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1d32pxv</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>International Nail Products in the US?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d32pxv/international_nail_products_in_the_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1d32k4z</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freestyle nail art </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d32k4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1d32cnp</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Can’t believe I forgot to share this vibrant set!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d32cnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1d325ud</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would these be considered velvet nails? </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d325ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1d31v5k</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Aurora nails</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g9fqjsyf3a3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1d31ph2</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Do my nails look pretty with this design?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d31ph2</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1d31mi1</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder Gel Suggestions </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d31mi1/builder_gel_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1d31e7z</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Getting into the *blursed* aesthetic</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d31e7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1d31d78</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Summertime blues 🩵🦋🌈</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d31d78</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1d316kc</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Did my nails!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uttcycmfx93d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1d3100s</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>My first time doing character art!</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3100s</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1d30va0</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Taco Bell theme</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d30va0</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1d30d5m</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cursed nail jutsu </t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d30d5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1d30d4j</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Hat Match</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d30d4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1d30d00</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d30d00</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1d302av</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>New colors!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d302av</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1d2zwt5</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>DND Loss Lavender with white chrome</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2zwt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1d2ztut</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Long nails make life fun for sure 💅🏻 @long nails alicia amira on google</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibe3s2hmk93d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1d2ze8j</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Is it too weird to provide my own Gel X nails at the salon?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2ze8j/is_it_too_weird_to_provide_my_own_gel_x_nails_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1d2z8wx</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Does anyone else’s chrome chip???</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqlkhtw3g93d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1d2z5ay</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Cute jumping spider fwend, and pretty nail polish.</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2z5ay</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1d2z20t</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Did a lil beachy set</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2z20t</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1d2z1kt</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Birthday nails with my birthday flowers!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otcuhgide93d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1d2yzq9</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>I'm a fan of pink so I love these designs, anyone else?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upxwuptwd93d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1d2ywoa</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>☯️</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muts6p68d93d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1d2ytke</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Showing off my nails AND my hamster </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4xmue3hc93d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1d2yn1x</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is $68 too much for this? Dip powder on real nails </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2yn1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1d2yj6x</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>My US Memorial Day Nails!</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2yj6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1d2ybz6</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>It’s my 6 month anniversary (with my nail tech)</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2ybz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1d2y7nw</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Love a fresh set!!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2y7nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1d2xdbl</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>My favorite color is pink, who team barbie 😍🤭</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rssnxzpm093d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1d2xc3k</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Tiniest lemon slice for summer</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zunw2ad093d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1d2ww6j</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Im in love 🩷🪩</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8t8asoww83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1d2wqyk</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>idk what to think about my nails... is so 2015!??</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cavzexjqv83d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1d2w78m</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Love a good white set 🤍</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cgaycair83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1d2w2e5</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Evil Eye Nails!</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2w2e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1d2vyar</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Would short almond work?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6aucyshlp83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1d2vg1h</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Haven’t done this in a while 😅 I regret not doing a solid color now aha</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2vg1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1d2vfiz</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>can’t believe these r press ones</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2vfiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1d2v9p0</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Is there any sweeter word heard than…</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2v9p0/is_there_any_sweeter_word_heard_than/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1d2v1mp</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>First attempt of acrylics on self</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5c785qati83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1d2ut0o</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>I loved this color</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w3o8rx2h83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1d2urwy</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>I’ve been doing my own nails this year and I feel like I’m getting the hang of it</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmn9hfkug83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1d2tq4n</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Is Gel-X the same as Apres?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2tq4n/is_gelx_the_same_as_apres/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1d2togx</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>I love stars ⭐️ ✨</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2togx</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1d2tlck</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>I got french tips. Wanted to go extra like u/Ok-Bed6354 but plans changed and maybe next time.</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ewr08ae883d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1d2th6h</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thank you to everyone who helped me yesterday 💕 </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7n8q8ekk783d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1d2t9tl</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>short and pink! perfect!</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtfdmqz6683d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1d2rwxq</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Orange &amp; pink...too lame?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2rwxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1d2rweq</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Cracks on dip powder</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79svtufvw73d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1d2rmyt</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Cherry bomb</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2rmyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1d2rdc0</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute spring time nails </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2rdc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1d2qwyz</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Second ever Gel x set on myself!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2qwyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1d2qosh</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Tried this shape for the first time</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2qosh</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1d2qg6e</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love w this set! </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0y21zihm73d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1d2q360</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>You can never go wrong with red!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4p2rv2mj73d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1d2ps8t</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went way outside my comfort zone with these, but I love them! </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ch15mjqh73d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1d2pksq</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Guess which nail is an exertion</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2pksq</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1d2pclw</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Pointers for doing gel nails?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/es4smh9ke73d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1d2p72z</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>The most expensive nail I got so far! I spent a little over $10 on this one and also the first time I went for bold color and big design.</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7or9mm8gd73d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1d2oyyt</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Pretty pretty office nails</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2oyyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1d2odou</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this thin "perfect" black line on my nail a splinter or something serious, what would you say? </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wos88k4f773d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1d2o9ws</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Growing acrylic out new mani 💅</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2o9ws</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1d2o9tn</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel X ? </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2o9tn/gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1d2o1nv</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>I love having my nails match my miniatures</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2o1nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1d2nuwu</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Gel polish after years of nails</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2nuwu/gel_polish_after_years_of_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1d2nn70</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flicker 🕯 </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2nn70</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1d2nhym</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>I ordered them short but they were thick, how can I lose them?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2nhym</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1d2nd88</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Made this set to celebrate the weather bring better</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2nd88</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1d2nd4f</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Made this set to celebrate the weather bring better</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2nd4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1d2nb8j</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Me and my nail tech’s newest creation</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2nb8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1d2n2ba</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you apply gel x nails with something other than nail glue? </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2n2ba/can_you_apply_gel_x_nails_with_something_other/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1d2mxne</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Perfect match with what I'm wearing today!</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukj7wgznw63d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1d2mwft</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail salons charging extra for acrylics PLUS gel instead of one price </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2mwft/nail_salons_charging_extra_for_acrylics_plus_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1d2mj34</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wedding nails for someone who knows nothing about nails. </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2mj34/wedding_nails_for_someone_who_knows_nothing_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1d2lx7x</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have a question </t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2lx7x/i_have_a_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1d2lwrl</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Got mine done for the first time in a long time this weekend. Just loving them ❤️</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zonh4q0uo63d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1d2lqcf</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Is it a winter or summer design? what do you think?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3qekb8hn63d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1d2lelq</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French Chrome </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2vz49n1l63d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1d2kg6n</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pastel Goth nail Art </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11tc3h8nd63d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1d2jw0j</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Cherub set done by my bestie!❤️</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gaptr1x6963d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1d2jm8l</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Beginner Nail Tech</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2jm8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1d2jafp</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>my first set of press on nailzzz💅🏼</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o72xbdn5463d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1d2j7vl</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2j7vl/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1d2hzr0</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I went on a press on nails shopping spree </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2hzr0/i_went_on_a_press_on_nails_shopping_spree/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1d2hz5s</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Traditional Tattoo Nails (done by Me)</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2hz5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1d2hu44</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Press-on Nails: Help Needed!</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2hu44/presson_nails_help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1d2h4d3</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Popart/comic nails! </t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2h4d3/popartcomic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1d2gd4z</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Am I in trouble?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hn22pheb53d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1d2gbuq</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to do gel polish art using non dominant hand </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d2gbuq/how_to_do_gel_polish_art_using_non_dominant_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1d3612b</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My bday 🎂 set 🥳 </t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3612b</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1d34tbg</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>My perfect summer color - Stolen Ambrosia by 🌙🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d34tbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1d34c46</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Replacement Brushes for Cirque</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d34c46/replacement_brushes_for_cirque/</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1d32vp8</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>I'm looking for recommendations for gorgeous chrome powders!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d32vp8/im_looking_for_recommendations_for_gorgeous/</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1d2zpbp</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Fake halo 🌈</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2zpbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1d2yj9a</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Help me pick a color!</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncd5pxl4a93d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1d32jf6</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>My first Mooncat order!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70e02eoeaa3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1d32hxm</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new favorite 😍 </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d32hxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1d31yv9</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Holy shift!</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jy0qfz2v4a3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1d30opu</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Cheshire Cat from Mooncat is so gorgeous!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ui9mr62us93d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1d306ea</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>All gradients, all the time</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d306ea</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1d2z40s</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute jumping spider fwend, and pretty nail polish. </t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2z40s</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1d2z29m</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Heard we were doing shimmer skittles ✨</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvhpe14je93d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1d2ymq8</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Saw it, immediately needed it</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2ymq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1d2ygxl</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Good vacation polish?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d2ygxl/good_vacation_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1d2y0d4</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Feeling like a plain Jane.</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2y0d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1d2xza1</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>first ilnp AND first time using a magnetic! 🧲 ✨(more pictures in comments)</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rplw1fs3593d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1d2xs08</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Crackle polish</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d2xs08/crackle_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1d2xrmo</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Bf said I have too many oils!? What are you HG nail care products?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2xrmo</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1d2xkki</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Bought a new polish to match my new car</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk9ouiz5293d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1d2woov</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Devastating</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2woov</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1d2wnje</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Glitter</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2wnje</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1d2wh67</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Clionadh Lux</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2wh67</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1d2wa6a</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>I've really been into candy pastels with splatter lately</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2wa6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1d2w73b</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Did I do good boss???</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c045t1rgr83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1d2v3tk</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Bee’s Knees - Little Star</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2v3tk</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1d2v0e4</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>“Are Mermaids Not Sweet?”</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2v0e4</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1d2ult9</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do my nails look like they're still growing, iyo? I'm having a really hard time telling and I've been squinting at these pics for a hot minute, lol. Same hand 2 weeks apart for comparison </t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lm57rxsmf83d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1d2ufyx</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>🌿🔮 Phoenix’s Ivy! 🔮🌿</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ktu96g1he83d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1d2u22r</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Please help me find a dupe!</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2u22r</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1d2tw7x</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>I tried *so hard* to give myself the picture perfect red mani. But woke up with crinkles 🥲🥴 I have decided I'm over it, lol. I am not perfect, and I tried my best. Life will carry on</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4k0bs5aja83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1d2rayq</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Mermaid Dreams 🫧</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2rayq</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1d2qute</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Best Reflective Topper?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d2qute/best_reflective_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1d2q425</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Easy space nails are the best</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2q425</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1d2pi40</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I call these safety hazard nails ⚠️ </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2pi40</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1d2ph2f</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>The fingers are a little dry because I've been working on my miniature displays, but I've been missing my nails having polish on them 😁</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90f28pcgf73d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1d2pg3i</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Taro Tea Wannabe</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qlrfbka8f73d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1d2p5vf</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Purple Flowers</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2p5vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1d2onhn</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Can I get a dupe or layering info on how to recreate this polish?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecrxacjh973d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1d2ogqc</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Is it normal for indie brands to have their websites down?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d2ogqc/is_it_normal_for_indie_brands_to_have_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1d2nfio</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🕯 </t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2nfio</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1d2nbl5</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blooming Azalea 🌺 </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2nbl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1d2n1up</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone ever try eyeshadow with a clear top coat? </t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y5cpq8ix63d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1d2ltpr</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I didn't think it would happen to me, but out of the 18 polished I ordered from mooncat, 1 broke. </t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2ltpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1d2lbre</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>🩵☁️Power Lines🐦💙</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2lbre</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1d2kvad</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Trying out Rubber Base Gel</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2kvad</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1d2kqkg</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Can anyone please help me find a polish similar to Essie "fawn"?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2kqkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1d2k87q</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Seafoam green with multi glitter</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3yy55qxb63d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1d2k7o8</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Jumped on the Flower Child bandwagon ✿</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2k7o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1d2ivub</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Rainy Spring Mani</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxf5snws063d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1d2ht7l</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Traditional Tattoo Nails (done by me)</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2ht7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1d2d57z</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Tried out my first holo polish!!</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckeqfwb5643d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1d2e432</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Sally Hansen Blue Serenity</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2e432</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1d2gyao</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>A total amateur who just LOVES glitter !</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6y1l0gyh53d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1d36cn8</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>I think these are the most beautiful nails I've made 🥰</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcl3p6jwhb3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1d36556</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>It was worth the time it took me to paint, these are my finished nails🫶🏻💖🧸</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdz8z3v9fb3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1d31z9w</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>ISO a vintage nail polish</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d31z9w/iso_a_vintage_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1d2z6sm</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freestyle Set </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xh9yd7mf93d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1d2yayn</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Had so much fun with these</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ie3bcr05893d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1d2xacq</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like ? </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5ff3bl0093d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1d2wxmj</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Ready for the Haikyuu movie 🧡🖤</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1mv6xz7x83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1d2upyj</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Some Chili Checkered Pressies I made a year ago! 🌶</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sysnbwagg83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1d2u7gw</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my first nails, Chameleon effect </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55ue9dsrc83d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1d2tftz</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Shoutout to my angel client!!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2tftz</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1d2o64r</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Encapsulated flower french (by IG: juun.yc)</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2o64r</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1d2mb25</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Tips to preserve gel polish on a palette??</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d2mb25/tips_to_preserve_gel_polish_on_a_palette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1d2jg2j</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Getting more into hand painted designs</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ffe301g563d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1d2iq1k</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Original art by me</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpu925kcz53d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1d2huz9</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>"Today, I want to try a punk style."</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2huz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1d2gsf3</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Star struck set </t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzaybbs6g53d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1d2eyzq</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Duck nail press ons. This is my first attempt.</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2eyzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1d2et5e</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>There’s 2 broken nails with temporary fix. Can you tell which ones?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d2et5e</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May 30 08:09:34 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_02.xlsx
+++ b/data/2024_06_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C644"/>
+  <dimension ref="A1:C823"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11381,6 +11381,3049 @@
         </is>
       </c>
     </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1d3ypye</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Gel polish on Natural Nails</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lbxmrwksi3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1d3yf3n</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>baby blue and chrome … can you be obsessed with your own hands? 😂</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsbveb4ioi3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1d3xqr9</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Cows. :3</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3xqr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1d3xpcy</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>My 4th set done by myself 🥹</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3xpcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1d3wes9</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>I did my own dip today</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3wes9</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1d3ghvm</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Just wanted to share my new set done by a new nail tech!</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3ghvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1d3vvh7</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>pretty pretties!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mav3vqfjth3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1d3v3sc</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Dip over my natural nails 😍</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3v3sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1d3ut5q</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>self manicure on biab extensions</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3ut5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1d3u8vu</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Acrylic Alternatives</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d3u8vu/acrylic_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1d3u4ev</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Lovee!</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kog26q8tbh3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1d3tw0s</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Summery Watermelon 🍉</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k24tdzxn9h3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1d3tqys</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Me feel Bonita 💖</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3tqys</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1d3tj7h</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>graduation nails</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkyeejad6h3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1d3thbf</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have nail beds that are so small they're almost round. I also play the ukulele and can't have my nails too long. I love manicures but regular nail polish only lasts about a day before chipping. Have any of you tried nail stains? Would that be a good option for me? </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d3thbf/i_have_nail_beds_that_are_so_small_theyre_almost/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1d3t8ok</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Chrome on natural length</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3t8ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1d3t5us</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>My baby hands got elongated almond lol</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3t5us</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1d3t45o</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>favorite set so far, happy almost pride!🤍</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3t45o</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1d3pnli</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Did these awhile ago but still love them.</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3pnli</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1d3rtx2</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t xml:space="preserve">April ‘24 </t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3rtx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1d3rjsg</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Groovy nails 🕺✨</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3rjsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1d3rgsi</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Cute set with a little heart. I love it</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s64qdelong3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1d3r9v6</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Nail guide?</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d3r9v6/nail_guide/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1d3r7zm</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love this polish </t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3r7zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1d3r57y</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Cutting my nails short soon for hobby reasons 🙏🏻🪦</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3r57y</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1d3qz88</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Neon green</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvkr1vb9jg3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1d3qsph</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>🎾 nails</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3qsph</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1d3qpck</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Cruella nails! What do you think!?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3qpck</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1d3q83t</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Last Week's Nails</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3q83t</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1d3q46q</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Wedding nail design ideas?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnhrokgubg3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1d3pwh1</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>shelliessss 🐡</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4y9s810ag3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1d3pra0</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Anyone else’s 2 hands so different nail wise?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3pra0</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1d3ogtx</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Nail supply sold me MMA monomer marketed as “no mma”</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d3ogtx/nail_supply_sold_me_mma_monomer_marketed_as_no_mma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1d3o335</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Green moment 🐸</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3o335</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1d3o19p</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loved doing and wearing these </t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21zvwxtuuf3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1d3nvl0</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Never ask to see my other hand</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4adj4nwptf3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1d3npzt</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Sticker nail tips</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwtn3xbjsf3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1d3nida</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Big Glowing Dill 🥒</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3nida</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1d3nhi8</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Press ons for the week 🌸</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3nhi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1d3n9fb</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons! Started wearing them to help me stop ripping and picking/nail biting at my skin it helps so much!! </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3n9fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1d3my41</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Update on the bad mani…</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3my41</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1d3mjx3</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Lavender Nails/Advice</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q61eslsif3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1d3mi25</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glamermaid butterflies </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3mi25</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1d3m1cn</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Price difference in uk to USA </t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d3m1cn/price_difference_in_uk_to_usa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1d3lytl</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Too pointy?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3lytl</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1d3lt4e</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand painted blinged out teeth nails </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3lt4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1d3ls57</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>french tips for mother’s day!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3ls57</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1d3lmsd</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Mint Green Press Ons</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3lmsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1d3lhg0</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Did my nails to match the cicadas’ eyes but I couldn’t find any to pose with :(</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yy2glbqv9f3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1d3l43r</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best press on nail glue? </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d3l43r/best_press_on_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1d3kym1</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>first time applying acrylic, tips for improvement?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnyookht5f3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1d3ks1g</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>What type of nails?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d3ks1g/what_type_of_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1d3kn1q</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Yet another french</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5qclxob3f3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1d3k2dd</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>First time getting my nails done in years</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3k2dd</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1d3k1fd</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>We need to talk about Cursed Poses…</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d3k1fd/we_need_to_talk_about_cursed_poses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1d3jo35</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Summer vibes with my cloud nails</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3jo35</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1d3jdy0</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Set for vacation 💅</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/im2lpbtmte3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1d3iv7z</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Matched my Nails to my DS</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3iv7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1d3imu1</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Simple nail art 🍃</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3imu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1d3ikfw</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Didn’t know what to expect with this color.</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0t3ldnjne3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1d3ifhz</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>birthday nails</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1eb5td5lme3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1d3i7tc</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>New Set!</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agj0k68zke3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1d3i6xn</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel this these are sci-fi aestheic claws </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpff0zmske3d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1d3hxnw</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>New Nails🦋🦄</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3hxnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1d3hk8p</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Oh so we’re doing abarbie manis now? I’m in!</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/VF9rXGz</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1d3hemc</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Vacation nails 🌺</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3hemc</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1d3hcyo</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>the French girl is always beautiful! and those relief drawings give it the special touch!</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q20exb2jee3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1d3haip</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple set!! </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40b2uaj0ee3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1d3gzim</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Long time no update</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3gzim</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1d3gxlw</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>I heard we are doing odd nail poses.</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3gxlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1d3g8dq</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Can you tell what this is supposed to be?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4t19n4iv5e3d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1d3f7mq</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Decided to be Barbie Brave</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3f7mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1d3ewch</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Summertime</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjf3l2snvd3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1d3ej1r</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Gel Nail easy removal?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjcu8xbwsd3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1d3e704</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>pressies &amp; a slight cursed pose</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pg6uaj4fqd3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1d3e4vv</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>aura nails — faded like crazy!</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3e4vv</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1d3ds1i</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>🥰🥰🥰🥰</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3ds1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1d3dmdc</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Nail art stickers/appliqués</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3dmdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1d3dlbs</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>spring-summer diys</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3dlbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1d3cnk2</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Best nail shape and length for fat short fingers</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ak4ht0uced3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1d3ck55</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Nails I've made this past year</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3ck55</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1d3c0bg</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>First time using press-ons featuring my cat 💖</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggya97k29d3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1d3bvge</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>How long does it take your nail tech to do your sculpted acrylics?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvxnz49w7d3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1d3btce</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Daughter's summer nails 💅</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ozvh6zd7d3d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1d3bt8z</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>As my daughter says, this set was “sooo lion king”</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebtdfpkc7d3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1d3ak04</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Sun moon and stars</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3ak04</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1d38yn9</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>How to get rid of my dark skin around cuticles?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d38yn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1d38tmi</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>3D Pool Water Nails</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d38tmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1d38jns</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Usually love pink but not digging these on my skin tone</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d38jns</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1d37rdl</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Lilac (?) jelly nails - love them!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d37rdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1d37glh</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>So in love with this set</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d37glh</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1d3wf7u</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>What colors usually suits warm toned fingers?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d3wf7u/what_colors_usually_suits_warm_toned_fingers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1d3vwsw</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is your favorite nail polish brand? </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d3vwsw/what_is_your_favorite_nail_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1d3v8t2</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>I bring you a beautiful winter color, I love how it looks</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/la1r495vmh3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1d3uto2</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>What do you think?? 🙈🫣</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3uto2</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1d3ueov</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nearly nekkid nails </t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0o3vm2leh3d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1d3tz39</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>My first Mooncat haul!🌙🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4zccqkfah3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1d3nnnn</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer - Moonbeam (May 2024 PPU)</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aeqisgx2sf3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1d3kns6</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>my What’s Up Beauty Memorial Day haul!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lawq55h3f3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1d39grl</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does any morrocan know from where I can get a professional e file bc I ‘ve searched there’s no supply </t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d39grl/does_any_morrocan_know_from_where_i_can_get_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1d37080</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can my nail beds grow back? It's short and pointy I want them to be round shape </t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d37080</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1d355fa</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Mooncat Thermal</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d355fa</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1d3tq05</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Cuticula skittle</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8b5ivi38h3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1d3thcw</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Poison.</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.imgur.com/a/i4QFTDX</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1d3su46</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Latest design I did!🦋</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3su46</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1d3sq1z</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's normal to keep the box... Right? </t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xq16rjb0zg3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1d3setf</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Stumped vs "Stumped"</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3setf</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1d3r59d</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>My overly dramatic cuticle oil bottles (for when you’re a Victorian vampire but still need to moisturize)</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3r59d</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1d3qz17</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Y’all already know 🌸</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5o2yuzk7jg3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1d3qyep</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Would it be too weird if</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h54w292jg3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1d3q6ra</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>How to stop skin picking/cutting?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3q6ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1d3pwkv</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Lilac You Meant It</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3pwkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1d3potp</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>The many colors of Freshly Bitten from Mooncat. I’ve never received so many compliments!! Just got this from the sale and am so in love with the formula.I had my doubts but they were dashed… dashed like so many other Mooncat bottles…</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tumm2jm58g3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1d3phj7</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Best toppers?</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d3phj7/best_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1d3pgh4</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Love me some nail jewelry</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbul3ff76g3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1d3p43j</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>I’ve been influenced</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3p43j</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1d3nvrd</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>How to maintain cuticles, skin and nails well even if they are short</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d3nvrd/how_to_maintain_cuticles_skin_and_nails_well_even/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1d3nkwz</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Big Glowing Dill 🥒</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3nkwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1d3mdvn</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Mermaid vibe combination</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3mdvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1d3m9mi</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>No polish allowed at my new job</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofdruqubgf3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1d3m7wi</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>One Giant Leap for Otter Kind</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3m7wi</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1d3m7gn</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Thermals are so hard to capture! (Photo 3 is my favorite!)</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3m7gn</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1d3l7lf</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>ILNP Skittle!</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3l7lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1d3l2du</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>First time using a magnetic!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtbaf2tm6f3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1d3kg4h</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>stencils featuring Abomination Cosmetics (on etsy)</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpsycigs1f3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1d3kdao</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>I am obsessed with iridescent flakies now ✨✨</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vaui44451f3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1d3k5rm</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Splash Talking</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3k5rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1d3jymf</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Thermal 💚🩵💙</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3jymf</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1d3jp2b</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seche Vive Gel Effect Top Coat </t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d3jp2b/seche_vive_gel_effect_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1d3ji9f</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about UV topcoat and Mooncat lacquer </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d3ji9f/question_about_uv_topcoat_and_mooncat_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1d3jf2l</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using gold foil </t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2csda0dvte3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1d3j748</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Lavender haze themed nails ✨</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qs8scfx6se3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1d3j6m4</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Trying to take a cute pic of my Mooncat nails with my cat - she was not amused</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3j6m4</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1d3izar</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>ILNP Willow 🌿💚</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3izar</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1d3iz3e</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>First time using magnetics</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3iz3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1d3isjq</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Would someone help me find a dupe for Londotown Kur "The full monty"?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d3isjq/would_someone_help_me_find_a_dupe_for_londotown/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1d3hrpq</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>ALL of my Mooncat polishes made the journey— there’s hope for you, yet!</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlr0zvplhe3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1d3ha6z</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>What I asked for v/s what I got !</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3ha6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1d3h9vo</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Butterfly spring nails</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7ejysysde3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1d3ev52</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Does anyone know a nail polish version for this eyeshadow?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3ev52</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1d3etqw</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Pass Me the Joystick - Watcha</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3etqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1d3e4cw</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This thermal kinda reminds me of the beach </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3e4cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1d3dqju</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Got two shades of blue in chrome</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3dqju</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1d3d8s9</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Fairy dust by ILNP being magical</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etf3u7eyid3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1d3d7po</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>This polish has me in a chokehold. Idk how I'm getting anything done today!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3d7po</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1d3d4eg</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>my mooncat treachery in the blue dupe✨</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3d4eg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1d3cqkq</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>May manis - ft Ethereal, Mooncat, and EdM</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3cqkq</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1d3cg9q</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>this is a sad day</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3cg9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1d3bjzl</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flakie Toppers: Mooncat vs. Holo Taco (or any other brands) </t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d3bjzl/flakie_toppers_mooncat_vs_holo_taco_or_any_other/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1d3bdgf</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"Bottom of the Pool" super happy with how these came out </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3bdgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1d3bays</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>All these years later, I’m still enchanted…</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4q5vqfis2d3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1d3ag7l</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Help with dip powders</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d3ag7l/help_with_dip_powders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1d39yoy</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love prugly polish </t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uljwd8nzpc3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1d39lrg</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>I love this polish! (even if it takes 4-5 coats) Sadly I'm running out of it, and it's no longer sold</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71bcnoo3mc3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1d38g0r</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural nails shape </t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d38g0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1d388en</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>DAE rush home to try new polishes and then hate the combination?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d388en</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1d31ast</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>My new favorite 😍</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d31ast</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1d3xn2e</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Nail art by white_lotus_salon on Instagram, anyone know how to achieve this?</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qjvdpgfei3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1d3x9xh</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>New to Nail Art</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3x9xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1d3vlsg</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>vacation nails w/ my boyfriend's initial</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycn5xzymqh3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1d3vl7l</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Nails rose</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d3vl7l/nails_rose/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1d3uumd</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>What do you think?? 🙈🫣</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3uumd</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1d3upwv</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>a beautiful set combining colors and art! 😍</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vjgxahmhh3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1d3tosi</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Same style different colors ✨</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77hbimls7h3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1d3rbxc</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>My first cat eye set 🐱</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d3rbxc/my_first_cat_eye_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1d3qq4g</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cruella nails! What do you think? </t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3qq4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1d3pcfv</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Working on some pressons for me 💕</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3pcfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1d3my0s</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1st successful time! </t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3my0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1d3lufc</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Orange &amp; black combined is fire 🔥</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3lufc</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1d3lqjz</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Simple, how is this? 🥰</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7giphhlubf3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1d3le15</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>press on set by me</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3le15</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1d3kpkn</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>I did a coquette set, turned out nice :)</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@soofs_nail_art/video/7373363613014297889</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1d3k8ej</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>First time doing nails! I started doing gel x nails on me and my family and these are the results!</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3k8ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1d3j1f3</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>a set that I loved making 💫</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izwuy4kzqe3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1d3ign2</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>New flower set by yours truly</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d3ign2/new_flower_set_by_yours_truly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1d3icrd</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>The butterfly nail art, which took 8 hours to conceptualize and create, do you think everyone will like it?I plan to make it into a series.</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://ovellaglam.com/enchanted-forest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1d3e152</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>3 weeks growth</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3e152</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1d3an6j</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do my nails look </t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3an6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1d39mja</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Some Sailor Moon Inspired Press Ons! 💟</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovet13ndmc3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May 31 08:09:23 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_02.xlsx
+++ b/data/2024_06_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C823"/>
+  <dimension ref="A1:C992"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14424,6 +14424,2879 @@
         </is>
       </c>
     </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1d4p1xd</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>I wanna be a nail tech but i barely get clients :( is my work good so far? I’ve been doing nails for 4 months and i’m 15</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4p1xd</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1d4oo6w</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>How much would you pay</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4oo6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1d4ofe3</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>New nails for new tattoos 💓</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jbx2thu9p3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1d4nzpk</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>I’m in love with my new set 😍</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lskfm4rt4p3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1d4nsv8</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>How to price these?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4nsv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1d4njom</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Longest Nails I’ve Done</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p11si21zzo3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1d4mvhp</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>and pose and pose and pose and pose</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4mvhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1d4mv1t</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>strawberry candy nails !!</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d94tstmoso3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1d4lqnm</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Nails for my soon to be sister in laws wedding 🥰</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc5pdi0hho3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1d4llxn</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>I got fired as a client..I assume</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4llxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1d4lfh3</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Recent set ✨💖</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45kbo2mgeo3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1d4l2od</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>I was a chronic nail biter until 2 weeks ago. My nails are now long enough for some adorable press-ons 🥳</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2d1o08zao3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1d4k72y</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>June set</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4k72y</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1d4k2po</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>First time gel x</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0k8qb0w71o3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1d4k0kw</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Got them done today 💖</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4k0kw</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1d4jp3u</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Pride Nails 2024</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijib4pq2yn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1d4jf5e</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>H0t Pink Mess - Top Coat or UV Light Issue?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4jf5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1d4je22</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>How I experiment 💅🏽</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a1k0kmn7vn3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1d4ja2y</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Dip manicures</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d4ja2y/dip_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1d4j9h2</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>First nail painting in 5 years</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f820nd1un3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1d4j337</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Newest set!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4j337</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1d4isf5</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t59gls5ppn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1d4iqx0</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>hello kitty summer nails</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvvzq9capn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1d4ij3f</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do I feel like these don’t suit me . Is it the shape ? New to manicures . Any business appropriate style ideas . </t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dc9fg7rcnn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1d4ieik</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Natural nails!</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4ieik</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1d4i909</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic short sets are the best! </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f6foytwkn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1d4i89o</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>I got my first Russian manicure today and I love my nails… I’ll never go back.</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rs6tejqkn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1d4hz71</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Loved this beachy look I got for Costa Rica</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4hz71</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1d4hth7</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>🍨 Painted Polish Mint Chip Madness 🍦 Oh my goodness, this shade makes me so happy! Who's ready for summer? Mint chip ice cream is my favorite!</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4hth7</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1d4h92w</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmeh6pejcn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1d4h0nf</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Colorful french tip nails.</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4h0nf</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1d4gqts</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>This is the best manicure I’ve ever gotten</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4gqts</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1d4gq1x</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>My nail lady hooked me up today 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4gq1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1d4gpjm</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Mani type that won't ruin natural nails</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d4gpjm/mani_type_that_wont_ruin_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1d4gm98</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>How long should you wait before applying new gel polish?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d4gm98/how_long_should_you_wait_before_applying_new_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1d4gip9</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Giving me pop art vibes (BIAB)</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zq0jxc5k6n3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1d4g26p</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Touch of Neon</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtg1clxv2n3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1d4fjo0</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Top coat turned them blue, I asked for black. I am still happy :). What do yall think?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fy586zhym3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1d4fjlu</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude pink glitter baby blue tips 💙 </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4fjlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1d4fi5d</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Added a few charms, felt like it needed something more</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzr4arn4ym3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1d4fhie</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone ever ordered from the Orly website? </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d4fhie/anyone_ever_ordered_from_the_orly_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1d4feyk</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Bus stop nails</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxmfqqmcxm3d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1d4f6ga</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails ✨ </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4f6ga</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1d4f3vs</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Clean girl nails with a little kick?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d4f3vs/clean_girl_nails_with_a_little_kick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1d4f2xi</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Help! I need advice!</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d4f2xi/help_i_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1d4ec7l</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Went a little crazy with the charms</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4ec7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1d4e441</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>beetlejuice nails in may</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4e441</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1d4e1pw</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>🤯🤯</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4e1pw</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1d49874</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Trying something new</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d49874</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1d49syo</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Hi! I graduated cosmetology school in January &amp; found my passion for nails! ✨</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d49syo</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1d49znz</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Gel polish chipped off</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dc65tletql3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1d4aivs</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Help me find a neutral glitter polish, ideally 2-3 coat full coverage</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d4aivs/help_me_find_a_neutral_glitter_polish_ideally_23/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1d4b5fj</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Strawberry nails 🍓🙂</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhlowd3nzl3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1d4bdaq</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>First attempt at gel extensions</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4bdaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1d4dnhm</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>I just wanted to show off my nails somewhere</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4dnhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1d4dnha</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>simple lil set 🩷</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qy0nmb4oim3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1d4d1ac</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>I’m obsessed with nail decals!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4d1ac</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1d4d0ge</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Mix and Match Nail Art</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4d0ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1d4czit</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>funny bunny with pink/blue holo chrome 🍬</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4czit</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1d4cogx</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Manicurist won’t remove all BIAB for new manicure?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d4cogx/manicurist_wont_remove_all_biab_for_new_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1d4cgds</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Summer vibes?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5aqv7iii9m3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1d4ce7c</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4ce7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1d4c4ab</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Rate my nails /hj</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4c4ab</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1d4bzew</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8hpik0x5m3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1d4bwce</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t xml:space="preserve">made these mermaid tail with barnacles vibe nails 🧜🏼‍♀️🐋🐚🦪 </t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4bwce</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1d4bu9c</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Blue blue blue</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4bu9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1d4bkl3</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone have recommendations for a rechargeable nail lamp that has GOOD battery life and can actually cure thick gels? </t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d4bkl3/anyone_have_recommendations_for_a_rechargeable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1d4bi0y</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>My nails for The Eras Tour!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80jpt15a2m3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1d4bhbn</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Frog nails</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/willg5p42m3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1d4b232</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>My boyfriend says, seeing this nail art is like having real butterflies fluttering in the grass😍. I'm totally digging the story behind this nail art!</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4b232</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1d4aw3h</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Latest set</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4aw3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1d4ap07</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>New press ons</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4ap07</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1d4a4ih</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Cow print baby!</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4a4ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1d49yhq</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Is this normal??</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d49yhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1d49ju3</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>my current set 💍</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d49ju3</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1d49fbs</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Gel manicure chipping after 5 days...</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d49fbs/gel_manicure_chipping_after_5_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1d49enh</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>a classic french tip 💘</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d49enh</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1d495mu</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>I did both hands!</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xj3p8kp7jl3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1d48jxg</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>look at the nails my friend did 😍</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqhpc2coel3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1d48a3m</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got my nails done..think I should ask for my money back? </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkmu028ncl3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1d489wo</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Clown nails!!!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d489wo</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1d486x9</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Love hate relationship with polish</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d486x9/love_hate_relationship_with_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1d47ryi</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Not my cleanest paint job but I do enjoy the colours</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvp3wun09l3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1d47r5y</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Kiss Impress Nails</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d47r5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1d47oeg</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Star nails </t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d47oeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1d47gty</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Another Basic B French Tip 😆</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d47gty</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1d46wba</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Beach ready</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owsx1li52l3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1d46o56</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Pastel Yellow 🐝</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d46o56</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1d461r9</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>My wedding nails from a few months ago, BIAB 😊✨</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d461r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1d460fv</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm glad I can post my nails here!! </t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d460fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1d45ygs</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my nails, always 😍 </t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d45ygs</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1d45mi0</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>I thought I’d be bold and try a new color, but now I’m hating it.</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d45mi0</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1d45cmw</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Been a minute since I did my nails!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovnhx846qk3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1d45155</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cinderella or Frozen? </t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zpxu98mnk3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1d44ayj</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gezejanshk3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1d445gs</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>what nail shape would fit my hands best?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d445gs</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1d442bs</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Blossom &amp; Buttercup 🤍</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikvffmerfk3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1d44145</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Lemon nails!</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d44145</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1d435ro</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">And I mean in do all of my nails! </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntmkoizs7k3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1d42ox4</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpz3ayvf3k3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1d4obq9</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>This color is so pretty 😭</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h47odcwm8p3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1d4o3dp</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Nail stickers: A Total Gamechanger!</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4o3dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1d4nvkl</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Thoughts on this brand? I’ve never heard of it before &amp; found it under the bed of a hotel I’m staying in.</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c69hspg3p3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1d4mes1</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>infection?</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d4mes1/infection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1d4m2nz</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Lil’ jelly tulips! I wish I took better pics but people were walking by and I panicked</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4m2nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1d4kr69</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>[Advice pls] Hey y'all I'm a tradesman who thought it would be fun to paint my nails last weekend... turns out I kinda like it</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zrf82cf7o3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1d4jz6a</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Forgot to post my last mani! Had me feeling very springtime</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4jz6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1d4jyjh</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Road Rage</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4jyjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1d4jydm</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>What is your favorite basecoat for staining?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d4jydm/what_is_your_favorite_basecoat_for_staining/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1d4j4b9</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>when work is a dumpster fire but at least your nails are kinda cute</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07lsspunsn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1d4igrn</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Mooncat Success!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zajn9uhsmn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1d4i8f1</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Would this make a good skittle?</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhb11rzrkn3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1d4i21k</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Bottle size 😑</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d4i21k/bottle_size/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1d4hrvp</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>🍨 Painted Polish Mint Chip Madness 🍦Oh my goodness, this shade makes me so happy! Who's ready for summer? Mint chip ice cream is my favorite!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4hrvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1d4h4pq</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>EXTREMELY short nails appreciation!!</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4h4pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1d4h337</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>🤩🤩🤩</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/knn8byl5bn3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1d4gy9c</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>My favorite nails from May</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9n26a40an3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1d4glq3</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>king of the castle , king of the castle 😂🤌🏻</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4glq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1d4fff6</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>The type of support every lacquerista deserves</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4fff6</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1d4f3w0</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Help! I need advice!</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d4f3w0/help_i_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1d4etpz</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Tips for healing onycholysis caused by gel manicures?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nayxkm3sm3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1d4dqj4</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Tinting builder gel?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d4dqj4/tinting_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1d4d7u0</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Jelly gel polish applying uneven, even with multiple coats</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbonvm5efm3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1d4d46k</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Resigned to stumpy shorties</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d4d46k/resigned_to_stumpy_shorties/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1d4bp8r</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>obsessed with this combo 🪶</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4bp8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1d4b1c7</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>SOS! Help me like this color! ILNP Morning Dew</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d4b1c7/sos_help_me_like_this_color_ilnp_morning_dew/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1d4abhr</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Known faders</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhibnmmbtl3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1d4a5wc</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Dino egg from space</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4a5wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1d4a377</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>ShiftyDustyShimmerGlowRainbowSkittleWow🎉</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4a377</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1d49hes</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>A Mooncat Lunat Sale Success Story</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d49hes/a_mooncat_lunat_sale_success_story/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1d490t2</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Shooting Star 🌠</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d490t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1d48m7h</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Mermaid's Tale 🧜‍♀️✨️</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d48m7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1d481k6</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Another Broken Mooncat bottle :(</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zpapy1zal3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1d47t4z</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>💜🌻Sunflowers🌻💜</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d47t4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1d47lje</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Two week old Mooncat mani!</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6gxkv5m7l3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1d47fvs</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Reformed nail biter and I need help</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d47fvs/reformed_nail_biter_and_i_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1d47eev</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Hippy dippy flower power</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d47eev</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1d474ea</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>How to get the 5d nail decals to look "encapsulated"</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d474ea/how_to_get_the_5d_nail_decals_to_look_encapsulated/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1d471po</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Love this sparkle</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/73zrf2bc3l3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1d46y7m</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Orchid is my summer color</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqcxz9fj2l3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1d46dru</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Putting polish over topcoat </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d46dru</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1d466v1</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>First time Mooncat order</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d466v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1d45v59</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Orange You Glad it's Summer? </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d45v59</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1d45qae</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>EdM Written Invitation is my favorite on grey rainy days</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d45qae</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1d45ndx</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brands releasing rainbow colours for Pride and just profiting off it with no donations </t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d45ndx/brands_releasing_rainbow_colours_for_pride_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1d44ufb</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Goodies from Japan!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkpqi9g6mk3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1d42y4f</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Polish lost in mail?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d42y4f/polish_lost_in_mail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1d42blu</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>What base coat is best?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d42blu/what_base_coat_is_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1d40boc</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Overfiled Nails: Pain</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d40boc/overfiled_nails_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1d3z5df</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Dreamy Dreamland mani</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d3z5df</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1d4qeok</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>does anyone else not like press-on nails? It feels like hardly anyone talks about them.By the way, I want to share my latest cat-eye purchase!</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4qeok</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1d4pu98</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think? </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvs726jbrp3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1d4n6em</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Magical girl aesthetic</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfqhjgzyvo3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1d4mdbl</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Clown nails! IG @kimtinaaa01</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4mdbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1d4lpxs</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Does anyone know how to do this kind of nail art?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4lpxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1d4l7i2</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Gel polish freehand :)</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4l7i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1d4jxl5</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>I accidentally did the gingham wrong on one hand</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a00ghw7b0o3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1d4j5zt</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Newest set!</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4j5zt</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1d4gnz2</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>This hurt me a lot.</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tavflcus7n3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1d4da1t</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zw1ecmnsfm3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1d4d1ln</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Mix and Match Nail Art</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4d1ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1d4cy06</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Help with liquid chrome application</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4cy06</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1d4a5gc</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Couldn't decide on black or neon. </t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mndskiv4sl3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1d49ldi</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>The Nails Bae Glaze Chrome Powder Set. What you think ? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/reey3s6qml3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1d46d7d</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1uhh6ue5yk3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1d45bt6</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>I thought it was easier to draw by hand..</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6j5pibwpk3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1d44cen</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Flower</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c2xbka4ik3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1d40r80</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbj4l95lij3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1d40qx2</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Vintage flowers 🥰 by moi</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yrc08klij3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jun  1 08:07:45 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_02.xlsx
+++ b/data/2024_06_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C992"/>
+  <dimension ref="A1:C1171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17297,6 +17297,3049 @@
         </is>
       </c>
     </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1d5htn3</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>I can’t seem to get my hand into a cursed pose</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2yq77of0x3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1d5hko1</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Week old nails (just wanted to practice poses tbh 💅)</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5hko1</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1d5hell</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Dream catchers</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5hell</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1d5hc46</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>I tried 3D nails 🌊</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16jyq8q6uw3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1d5gk9u</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>first time getting charms 🦋</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5gk9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1d5gizz</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Did my little sisters nails</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pa3f70kbkw3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1d5gdno</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Light Pink Nails</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5gdno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1d5fwht</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>what does this mean?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wup8ktsxcw3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1d5frei</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Opinion on polish quality?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d5frei/opinion_on_polish_quality/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1d5fhmn</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Rate this nails</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5fhmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1d5fb1a</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Did French manicure on my own nails</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5fb1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1d5ehgj</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Something different</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avin36ohxv3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1d5e6ms</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>First time doing my nails in 3 years.</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5e6ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1d5e5w4</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>I am in love</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5e5w4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1d5e5ne</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>I am in love</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5e5ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1d5e5lb</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>First time doing my nails in 3 years.</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5e5lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1d5e4zx</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Wanted to show off my press-ons</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5e4zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1d5e39g</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>I’m such a Dazzledry diehard</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4cwcakntv3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1d5dpd1</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Do you like the shape?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5dpd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1d5dhtd</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>went to a new girl and she was able to take off my bio gel without ruining my nails and do this masterpiece on my natural nails!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5dhtd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1d5db4v</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>wanted to post my wedding/honeymoon nails!</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5db4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1d5d0yw</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Let’s get crazy</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7c7z6loiv3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1d5cyi4</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I bite on my cuticles and I rejected my nail care for a  long time , now I take care of them clean them up and color them . They look cute </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5cyi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1d5crom</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>My fave set I ever had 🥰</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5crom</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1d5cjj2</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>What do u think??</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6vzo0dsdv3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1d5ce27</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>I've never had nails that long</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41vvp8n9cv3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1d5cc83</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Super old hand me down, Lo'real Rythmn and Blue</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5cc83</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1d5caqv</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Shape</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlwxooocbv3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1d5c2h3</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Happy Pride!</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5c2h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1d5brwh</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>New nails 💙</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1fdiw786v3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1d5bjhc</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oh. Em. Ghee. Look at this! I know it’s a lil weird but it’s a lil amazing too! </t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/C7iC9XMsn7Q/?igsh=MTQ1cGF2a3Z5ejA2MQ==</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1d5bf36</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Me and my son got matching sets</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgnoe2vr2v3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1d5b7rc</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>pompompurin nails</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5b7rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1d5aqem</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Simple and elegant</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5aqem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1d5amdr</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>What existing color matches this base color? Any OPI colors?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ob225d36vu3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1d5aeu5</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Why do nail techs hate doing short acrylics?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d5aeu5/why_do_nail_techs_hate_doing_short_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1d5a92y</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>press ons i made for myself</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5a92y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1d5a8aw</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>“Soft” French 🤍🤍</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9j1e0doru3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1d5a7nh</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fairy nails 🧚‍♀️💅 </t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5a7nh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1d5a4f3</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>My nail tech called these cat eyes</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awa1hfqpqu3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1d5a1nq</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xlj0aw1qu3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1d59vt6</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Prob the set I'm most proud of..</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d59vt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1d59hg5</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticle care recommendations? </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpsg5dw7lu3d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1d524c7</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>OPI Press-Ons review: high quality but not for wide or large nails</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6gvuvupys3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1d533w5</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Nail tech slayed again!</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d533w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1d576so</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Do yall cut for file these? I only have a few nails like this</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kamnyk02u3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1d58d7i</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>First ever acrylics at home 🫣</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d58d7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1d59adh</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>First time doing nail art, design and inspo credits to @nailsbyalsn on Instagram.</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d59adh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1d5986m</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>First time at a nail salon early May and got some strawberry nails done</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5986m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1d58o1l</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>I wanted the jelly/nuance nail in jewel tones for my trip to Montana.. close enough!!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d58o1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1d58n20</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>fourth time doing gel x on myself :]</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d58n20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1d58c5h</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>The nail art i do for my girlfriend and I</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d58c5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1d585fr</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Press-on gang 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7bax6ot9u3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1d5840j</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Minimalist vibes 🤩</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n80mli6i9u3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1d583jm</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Got press-ons for the first time at a salon, and they look horrible underneath when backlit 😑</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d583jm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1d57qu6</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome powders + some cat eye for fun. 🤩 </t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqleo0sd6u3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1d57i54</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Wet N Wild-Be More Pacific, I had it in my de stash pile now im not sure lol</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d57i54</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1d579vy</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>fresh frenchies 💅🏽🤍</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d579vy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1d575e0</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Are metal glue on nails a thing?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d575e0/are_metal_glue_on_nails_a_thing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1d574m7</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Fruit nails for summer 🍓🍋🍒🍊🫐</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olglaq6j1u3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1d573sv</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Natural nails win!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2nzpbyb1u3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1d572p4</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>New Nail Day!</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d572p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1d57263</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Cornflowers</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d57263</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1d56n4e</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Second Attempt With Soft Gel Tips</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrsqoadmxt3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1d55wpq</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Best gel top coat that works with regular top coat?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d55wpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1d55wll</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>My first attempt at press-ons</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d55wll</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1d55c0d</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My second attempt </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d55c0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1d5593k</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Daisies are my favourite flower 🩷</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu6c9odqmt3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1d558wb</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>My first set of gel overlay! Should I redo before my 3-week trip?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d558wb/my_first_set_of_gel_overlay_should_i_redo_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1d55732</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Just for me</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d55732/just_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1d5568s</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>I need help</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5568s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1d54g6m</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>new set!!!</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d54g6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1d547qk</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Sparkly Iridescent natural nails</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d547qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1d54365</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Happy Pride!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d54365</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1d5420u</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Saying Hello to Pride Month with some trippy rainbow nails! Hand-painted on a polygel base</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3yt57ifdt3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1d53yeo</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>I love my new nails!</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d53yeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1d53vwl</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>my favorite that ive gotten in a long time :)</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sag88rg4ct3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1d53uyz</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>something different 🩷😍</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhuhgrywbt3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1d53p42</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Vacation Nails</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d53p42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1d53gs0</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>New set in love with the shape and the colour, thoughts?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i57ew2v8t3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1d53bi7</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>can i mix and match brands?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d53bi7/can_i_mix_and_match_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1d538oo</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Ying and Yang Nails</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fa6hzwga7t3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1d532kb</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Practice</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96za70hz5t3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1d52w2n</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Went to a new salon and I’m obsessed worth the $110.</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwoqhlcl4t3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1d52qma</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Probably my favourite set ❤️</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d52qma</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1d52o44</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Coffee with milk 🤤</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4q7i9qx2t3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1d52hjq</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Bright</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0lkg3zi1t3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1d52g44</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Is there any at-home substitute for Structured Gel Nails?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d52g44/is_there_any_athome_substitute_for_structured_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1d52ayg</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>I wanna get weird, too</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d52ayg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1d524so</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Trying to schedule a mani, but I'm not sure what to book or what it's commonly called - super soft nails edition</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d524so/trying_to_schedule_a_mani_but_im_not_sure_what_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1d51qo3</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Ocean Blue</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gc1y5hmtvs3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1d51nz7</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Manicure question for a newbie with long natural nails!</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d51nz7/manicure_question_for_a_newbie_with_long_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1d51lk6</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Hair Dye Disasters</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d51lk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1d51jr5</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>new nails i put on for my beach vacation! ❣️</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d51jr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1d51g3u</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Just fixed a devastatingly broken nail using dip powder and so far it’s holding and feels quite strong</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d51g3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1d518fs</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>cherry blossoms with some chrome</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d518fs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1d513y5</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d513y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1d50zc0</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What Do you think about my nails? </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d50zc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1d50vr7</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>I did my own nails</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/99fdwes6ps3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1d50nn3</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Latest mix and match set I did</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d50nn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1d5h4r3</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Anyone know what this is fooooor? My boyfriend is using his 3D printer to make these for me!</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alzkvtnorw3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1d5gu5l</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was sleeping on the 3.50$ Essence Holo Bomb </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5gu5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1d5gbgt</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t xml:space="preserve">silver polishes? </t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5gbgt/silver_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1d5f4mb</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Obscure</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5f4mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1d5f2lk</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Had to show it off</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hdu8hhjo3w3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1d5ez0k</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Phoenix Ivy</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5ez0k/phoenix_ivy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1d5e5ft</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Hey Mercury, Can You Not?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5e5ft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1d5e0y6</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Baroness X Octo-Alien</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5e0y6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1d5dqea</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>For those who have been looking for their unicorn, a bottle of Mooncat’s Supernatural just showed up on Mercari around 11pm EST.</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5dqea/for_those_who_have_been_looking_for_their_unicorn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1d5czk2</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>That glow tho</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5czk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1d5cuv2</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Important service announcement: my nail polish matches this frog</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdzbwxuygv3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1d5c37e</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>What to do with the old, skinny brushes?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bunk1pa9v3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1d5bvp5</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Queen of Rot 💚🤎💚</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5bvp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1d5brtz</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Final pics of this weeks mani before I take it off and start over!</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5brtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1d5booy</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Freshly Bitten // The Trouble with Immortality</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5booy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1d5boan</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just looked down and noticed that Sand Viper by Mooncat PERFECTLY matches my Jammies. Happy Friday! </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4y6v5xa5v3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1d5bmw7</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>house of hades my beloved</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5bmw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1d5b6ox</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>What I wore in May</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5b6ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1d5ae92</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Does anyone know of a nude regular nail polish as the one in this photo?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dcgxav7tu3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1d59mq0</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Check out this amazing polish that I totally discovered on my own and wasn't influenced by all of you to buy</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d59mq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1d58xv1</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PSA: nail polish deals at Walgreens </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d58xv1/psa_nail_polish_deals_at_walgreens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1d58xda</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>So shimmery and shifty</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d58xda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1d58jop</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Mom always know what to say to make me feel better, lol</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/617vugb7du3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1d57w1x</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Phoenix Ivy loooove ♥️🌿</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d57w1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1d57bmt</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>morning rays - ILNP ☀️</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5nm6bs23u3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1d57blg</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Cirque colors jelly skittle (featuring my husband)</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d57blg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1d570nk</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Cornflowers</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d570nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1d565ve</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish Remover </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d565ve/polish_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1d553ei</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Just obsessed</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d553ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1d54kpw</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Juicy jelly sandwich!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d54kpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1d54jq3</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Swatched my polishes from my first PPU and it seems my cat Bean is also impressed</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d54jq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1d54di0</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>What can I do to cover my ugly missing nail?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzz8hlayft3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1d5452b</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Space vibes and my first time doing magnetic polish!</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5452b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1d53n3j</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Can anyone help me ID this polish or similar? It’s gorgeous</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goofyq08at3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1d53bar</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Preventing Orly Builder Stains</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1t7nnlgt7t3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1d51xs5</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Eldritch Dream World</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d51xs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1d51r2i</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Has anyone tried this? 🧐</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96vqzj4xvs3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1d51nt4</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>The longest my nails have been in a VERY long time</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d51nt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1d51nl1</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">That’s what I’m talking ‘bout!! </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izbneux5vs3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1d51c04</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Am I the only one who can NEVER find the poll for PPU?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d51c04/am_i_the_only_one_who_can_never_find_the_poll_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1d51938</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Reminds me of Embers</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d51938</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1d50i7d</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>You can only choose one indie brand to buy from for the rest of your life. Which brand is it?</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d50i7d/you_can_only_choose_one_indie_brand_to_buy_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1d4zgkp</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Magnetic holo Fizzy Lifting Drink</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4zgkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1d4y5ul</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>👽🐄Beam Me Up🛸👽</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4y5ul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1d4xqda</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Terrible application aside, which of these two colors suits me more? </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9y6ov8va1s3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1d4xoyb</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Stenciling with jellies!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4xoyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1d4xb2k</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>I am so in love with Rogue Lacquer's Chai Latte ☕️ 🥰</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ernx4jivxr3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1d4wgjn</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Evermore is a dream</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tk6p36aarr3d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1d4vmpu</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice needed my mani never lasts </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3s92tgkkr3d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1d4uo33</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Broken nail as Accent! (Or: Lemonade from lemons)</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://imgur.com/D2Mzp9E</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1d4u194</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Sneaky accent nails 🤫</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbkqv3l66r3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1d4tx9r</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Last minute decided to try bright green tips. Phoenix - You Always Be My Sister</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4tx9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1d4trhx</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Elixir of Everlasting Life </t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4trhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1d4t6q5</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Definitely my favourite nails of the year 🩷🎀</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4t6q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1d4swqu</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Dress to Nails Inspo</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4swqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1d4su0t</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Why does my nails curve upwards?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d4su0t/why_does_my_nails_curve_upwards/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1d4ss5x</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>MOONCAT - Ultrahot 🔥</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9l8aj31tq3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1d4sq5k</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>First time trying decals</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl6jn83esq3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1d4se2s</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Nailtopia: Perfectionists. TRY IT.</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d4se2s/nailtopia_perfectionists_try_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1d4s466</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Chunky, reflective flakeys?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdja6f1xkq3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1d5hdo7</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Dream catchers</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5hdo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1d5fm5m</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🌸Hand painted🌸 Cherry blossoms </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jlveeim9w3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1d5fl3v</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel x done by me in bc Canada </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5fl3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1d5fig9</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>recent nails for a photoshoot!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5fig9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1d5f9z6</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Hello people!! what do you think??? Three months ago I learned how to decorate nails and I'm still learning!! Give me karma if you like to motivate me and continue learning more every day!! thank you!!!☺️☺️</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4274hhx5w3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1d5cdga</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Hand painted Strawberry Nails🍓💅🏼</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yydhhjf3cv3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1d5a8ad</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>press ons i made for myself</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5a8ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1d573ss</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Fruit nails 🍓🍋🍒🍊🫐</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asl103jc1u3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1d56lfg</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Some sets I done lately 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d56lfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1d565zz</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Question about making ombre nails with powder.</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d565zz/question_about_making_ombre_nails_with_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1d56210</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Other Jamaica flag nail art</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fs5kjb01tt3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1d52pvl</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Lovelovelove them 🩶🕷️</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d52pvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1d52dji</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Just wanted to share my pain with people who will understand 😩</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pk4f9so0t3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1d4wwau</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>loving the color red 😍♥️</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11wwq5nqur3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1d4wia8</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Throw back….Christmas nail design</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4wia8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1d4wf96</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4wf96</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1d4tta1</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Beginner at nails</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsdqohb14r3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1d4tlwv</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>These nails make me feel like a total witch! 🧙‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4tlwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1d4slcx</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Even though these press-on nails cost me 45$, I think they’re totally worth it!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d4slcx</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun  2 08:07:35 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_02.xlsx
+++ b/data/2024_06_02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1171"/>
+  <dimension ref="A1:C1353"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20340,6 +20340,3102 @@
         </is>
       </c>
     </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1d681cj</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>I cant push my cuticles back</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d681cj/i_cant_push_my_cuticles_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1d67p36</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Petri dish 🦠</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d67p36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1d5iicc</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Got french chrome for the first time</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5iicc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1d5jppb</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>How do I neaten these?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5jppb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1d5jy67</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>I made my favorite set so far 🐝🍓🐞🍋🌷</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5jy67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1d5tyu9</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Researching Specifics on how to get salon quality press-ons at home that stay for 2 weeks and how to get them off if you use protein primer + nail glue…</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4qmqv1bb04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1d5v4mw</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>New set (nail tech in training)</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zz2qpg0uk04d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1d65ni6</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which one for this summer? </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brxlyhn8b34d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1d66adv</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Help with basics</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78kj1uuri34d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1d62xgw</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>help me pick a manicure colour!</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d62xgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1d65fvf</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>I got my June nails just in time for the rainy season! ☔️</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d65fvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1d65w51</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Nail care for really soft/bendy nails?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d65w51/nail_care_for_really_softbendy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1d66gyq</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>love this design 💛</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oah83xywk34d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1d66eqd</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>I have so much love for getting my nails done. ❣️ and my nail tech is beyond amazing. 🫶🏽🥲</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d66eqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1d66cmz</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>We're these Worth $80? Should I go back?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6g6ncc4ij34d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1d65ohg</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>At home nail tech!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d65ohg/at_home_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1d65k8r</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>One of the hardest decisions 😬😂</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6kp3ms3a34d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1d65jzk</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Is there anything similar to structure but doesn’t need curing? I’ve stopped getting gels for a while but I miss the magic of that structure layer.</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d65jzk/is_there_anything_similar_to_structure_but_doesnt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1d65hhj</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Accidental matching 🤣😂</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zon81l7934d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1d652i9</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>This is probably my favorite design so far.</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubi8dine434d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1d6529z</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Sometimes it’s good to go with a baby pink🎀🩷</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d6529z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1d64q2h</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Graduation nails</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lefdl1m034d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1d64hsu</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Sunshine Yellow!</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ht5aym3y24d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1d64g9e</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My wife best nail </t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14paoofnx24d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1d64cuw</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Are these bad? What kind of nails do I have on?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d64cuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1d64aee</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Did press on nails help beat your nail biting and help your actual nails grow naturally??? I really don’t want to spend the money on getting acrylics every few weeks 🥲</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d64aee/did_press_on_nails_help_beat_your_nail_biting_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1d63uf2</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>New salon and my first time getting my nails done again</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d63uf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1d63qpm</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Not pretty nails and need help!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spaiu099q24d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1d63k0i</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel (no UV) vs regular polish </t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d63k0i/gel_no_uv_vs_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1d63gxe</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Press ons for a friend</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d63gxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1d63b3e</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>First time getting almond… thoughts?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d63b3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1d632gy</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Obsessed with my “artist’s choice” nails</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d632gy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1d62rmc</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Fairy set 🧚🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d62rmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1d62plv</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Bi Pride</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxp9xobof24d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1d62gw0</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Glazed French</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d62gw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1d62cl1</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Witchy set by me</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d62cl1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1d62c4q</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Great Magnet Strength</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3bz1353xb24d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1d62b7n</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Gel X</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d62b7n/gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1d629ci</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>this has gotta be a first for me</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbacpto4b24d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1d622et</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>NEED HELP PICKING A DESIGN TO DRAW ON PINKY!! Any ideas? *Florida theme*</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d622et</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1d61yt1</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Dazzle Dry love</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d61yt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1d61gsa</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>I’m literally obsessed with this set</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d61gsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1d61a62</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Before and After for my bestie ✨</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d61a62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1d605ff</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Summer nails I got done @ school</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d605ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1d601yo</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Press Ons - An Album</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d601yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1d5zv5c</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🐉 scales </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5zv5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1d5zhmt</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>This months set 😍</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03t2jr9el14d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1d5zhb4</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Ooooh witchy woman 🌙✨</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5zhb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1d5zfd3</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ll9b0qauk14d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1d5zcvz</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>in love with my Slytherin nails (glow in the dark teehee)!! lost one on a ride tho 😢</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5zcvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1d5z975</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Always shinning</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tcxgbzdj14d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1d5yxan</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Went a lil short for work and I kinda like the short vibes right now 🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5yxan</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1d5ypaj</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5ypaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1d5ylyz</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Finally mastered checkerboard! 💓</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bglqrqeld14d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1d5ykd4</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>How often is to often to re-do nails</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d5ykd4/how_often_is_to_often_to_redo_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1d5y0j1</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Requesting Refunds</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8egrefvr814d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1d5xy12</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My manicure for the summer :) </t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9zvlam7814d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1d5xxnj</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Moon Cat polish</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ibirkm2814d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1d5xdv2</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Fresh set for a fresh start. I start my new job Monday!</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehesiq9i314d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1d5xcmp</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Ready for June</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6xssnp7314d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1d5xbvl</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Are all of these products good enough?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpjuoao1314d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1d5xb2k</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Red nails are my favourite</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmvqvzzu214d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1d5x9a0</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>TGB BIAB equivalent?</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d5x9a0/tgb_biab_equivalent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1d5x89q</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>my nail progression ❤️</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5x89q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1d5x4hb</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>New Mani ☀️</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1a6fkyeb114d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1d5wxv0</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Soft Builder Gel</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d5wxv0/soft_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1d5wwzv</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Velvet cat eye coffins💨</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu9jle7lz04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1d5w7ul</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Some of my favorite nails I’ve done on myself</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5w7ul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1d5w48l</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>home manicure</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5w48l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1d5w1ab</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Do you like the color?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7dydat5s04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1d5w129</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Thoughts</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5w129</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1d5vze7</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>OPI Press Ons</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5vze7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1d5vrjr</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>A quick shimmery look for the weekend</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5vrjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1d5vdvb</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Nails for my sister's baby shower (it's a boy)</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5vdvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1d5v6p3</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Lifelong nail biter five months into regular manicures</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5v6p3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1d5v3ip</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Educate me!</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d5v3ip/educate_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1d5uz9p</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Cursed Toe Nails</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3uxvozmj04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1d5uy91</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>First time with cat eye gel polish</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5uy91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1d5uv5g</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Nail art</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5uv5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1d5utlc</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Would it be insane to just get fills with this color forever?</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acfe3q1bi04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1d5unnq</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Mermaid Bait is Delicious!</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5unnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1d5uiv7</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Love my sparkly summer nails</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn5xomusf04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1d5u1eq</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Bright red nails ✨</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5u1eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1d5u0l4</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Press on nails and painted toes 😙</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5u0l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1d5tcp4</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Favorite (pink-toned) nudes?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d5tcp4/favorite_pinktoned_nudes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1d5suy7</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>When life gives you lemons 🍋</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5suy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1d5sp82</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>I couldn’t stop adding pearls</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5sp82</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1d5snc1</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Almond shape, yay or nay? Done at the salon, do they look too thick and wide? Acrylic tips </t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifelf8no004d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1d5sgvt</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My third diy gel x set </t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5sgvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1d5sg02</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun summer design. </t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbb3xuvyyz3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1d5sccl</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>I did these during Xmas time. I thought you all might like them.</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5sccl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1d5s40a</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>🌈 ☁️ 🩷 priiiiide!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5s40a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1d5s3vi</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Todays client wanted fruit nails. </t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qa38rj46wz3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1d5s0v6</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>70’s vibes</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxu2richvz3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1d5rtgx</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Day 27 and still no chips!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5rtgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1d5rchu</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>First time getting nails done</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5rchu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1d5rb8h</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>pink chrome sunset 💖</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5eq3trdlpz3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1d5r7u8</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Really love this set</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79lutygtoz3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1d5quj8</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Another pic of my blueberry nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjv1ej7slz3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1d5qsgx</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Clean look ✨</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5qsgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1d65wcv</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>The dreaded destash mani</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d65wcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1d65j7y</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Been obsessed with texture</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d65j7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1d64mak</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Why does my nail polish have holes/lumps?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vb0thi6fz24d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1d64ae0</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>despite the shimmer and a glitter topcoat it’s still giving mannequin hands 😔</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/58d49z9wv24d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1d649pb</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Cat’s Paw by LynB Designs</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d649pb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1d63h2q</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Jelly Polish</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d63h2q/jelly_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1d63e77</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Playing around with ghibli stickers</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d63e77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1d633lx</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Shaky hands?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d633lx/shaky_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1d60d9y</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Inspired by a pic I found and Electric Daisy was perfect for it</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d60d9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1d5yx5n</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Happy nail polish day from my shorties and me :)</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5yx5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1d5ywzv</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Disney skittle on my kid</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5ywzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1d5yrow</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>What do you do with colours you don’t like on you?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yt1ck813f14d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1d5yo4x</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>My nails since April 1st</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5yo4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1d5yl9t</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Who is your favorite thermal creator and why is it Sassy Sauce?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56xdxfwid14d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1d5yisq</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Baby pink holo taco dupe</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5yisq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1d5yd25</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Pan Pride 💙💛💖</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5yd25</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1d5x6h6</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>My first time ever buying a full collection of nail polishes and I am so happy 🌈</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5x6h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1d5x048</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Aftercare after getting dip nails removed</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5x048/aftercare_after_getting_dip_nails_removed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1d5vvgo</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m not a cat, I don’t say meow 🐮 </t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuastn5rq04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1d5vusm</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Pride inspired nails for June? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yk727d6jq04d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1d5vec8</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>A ✨sparkle✨ mani to start June!</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u9gs5wym04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1d5upqx</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Review: Essie's Gel Setter vs Gel Couture top coats, here are my experiences with both and how they compare!</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5upqx/review_essies_gel_setter_vs_gel_couture_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1d5u80c</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>HAPPY NATIONAL POLISH DAY Cheers to healthy nails 💅🏾🩷</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uoj4zlkcd04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1d5u7oq</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Maybe it’s because I’m new to this…</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xe9ctxad04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1d5u3g5</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Nail Polish day! </t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5u3g5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1d588q6</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>French manicure</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d588q6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1d5tq78</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>do you like these colors?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhyw7hs9904d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1d5tkn7</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">National Nail Polish Day </t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjtmncw2804d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1d5swpz</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Take Me To Your Leader by Mooncat. Most slept on polish ever?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ntk34jo204d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1d5sqaq</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Anyone have that polish color they love, but the application is awful?</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5sqaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1d5s968</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Mooncat Base causing polish to come off in one piece?</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dejqrdsfxz3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1d5s7ix</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Mermaid For This ✨️</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5s7ix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1d5s1lc</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Happy Pride Month! Check out my take on a Pride design. Insta - @Charli.bell.9</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5s1lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1d5s0vc</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Vice watermarble for Pride month 🌈</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5s0vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1d5rzxe</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>💙💕 Truth or Dare 💕💙</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5rzxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1d5ruzr</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Anyone else make their own nail polish?</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5ruzr/anyone_else_make_their_own_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1d5rhpb</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Cirque xoxo vs ILNP Malibu</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5rhpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1d5r41r</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP metallic longevity? </t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5r41r/ilnp_metallic_longevity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1d5qh4u</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are some viable options for someone incapable of painting their nails? </t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5qh4u/what_are_some_viable_options_for_someone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1d5qg06</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>A pain in the Asteroid</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5qg06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1d5qdsq</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈🫶LOVE🫶🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5qdsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1d5q4ny</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>What are your thoughts on the Holo Taco Rock Candy Collection?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5q4ny/what_are_your_thoughts_on_the_holo_taco_rock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1d5px2b</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>When your mani is your hair inspo</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4b4g8d9ez3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1d5pn4i</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fave products </t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5pn4i/fave_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1d5pklj</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>You Are Not Alone</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5pklj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1d5pecd</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Help me choose my skittle</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5pecd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1d5onfe</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>it’s National Nail polish day! i’m celebrating with gorgeous painted nails but i’d love to know what is everyone’s favorite polish?! il post mine!!!!</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mf1u1s3v3z3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1d5okx0</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>National Nail Polish Day!</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5okx0/national_nail_polish_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1d5ojbi</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Bi nails, babyyyy. 😎</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5ojbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1d5o0qk</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Have you ever loved a polish, decided to do some stamping…</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5o0qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1d5nts2</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Tried my first dotticure today!</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5nts2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1d5ngh1</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>strawberry milk 🥰🍓</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lz448yuoty3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1d5najf</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Such a fun thermal 😍</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15xca687sy3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1d5n5d3</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>This is STUNNING!</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5n5d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1d5lphp</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Thermal Love</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5lphp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1d5lj5f</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>What I wore in May 🌸</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5lj5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1d5kya5</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>The shift is incredible 😍</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.imgur.com/a/TTlvKGM</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1d5jxbj</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Recently got back into nails and discovered layered stamping. I can’t believe these are my nails, I want to frame it they’re so pretty!</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0kxwzr1sx3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1d5jnvt</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5jnvt/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1d5itkc</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Swatch request - Ethereal's Siren collection</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d5itkc/swatch_request_ethereals_siren_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1d50vqh</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers Haul</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d50vqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1d66k1z</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which one for summer? </t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqd8i9ryl34d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1d66czg</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>My nails with a new design, how does it look?</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4fpymamj34d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1d66cb2</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>different design 🤩</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n96flqwdj34d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1d64bry</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Nails for graduation 🩷</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d64bry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1d63aw4</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Mermaid chrome</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yewah7aol24d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1d62ewx</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Can anyone help me pick a design to draw on pinky? I’m doing florida themed nails!</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d62ewx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1d61s28</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Chrome tips...on Diami Oh'ver Gel</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d61s28</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1d61rkk</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>First Set</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d61rkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1d5z84x</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Lucky charm 🍀</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fi8guz34j14d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1d5yzxd</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>I just love practicing nail art 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5yzxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1d5xz1h</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>summer smiley set! :) :) :)</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5xz1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1d5wpmc</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>My favorite set I've done</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5wpmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1d5wjoj</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>latest press-ons</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k165cuehw04d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1d5vkc0</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Happy Pride :) (OC)</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5vkc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1d5t6wg</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>This bow is more secure than I imagined.</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5t6wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1d5s6gs</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Happy Pride Month! Check out my take on a Pride design. Insta - @Charli.bell.9
+</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5s6gs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1d5pl8w</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>The Nails Bae Silver&amp;Gold 3D Set. IG@ NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8gn2zkkbz3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1d5p530</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Summer colorful french☀️</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/639x56hw7z3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1d5nwas</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1i5e9blkxy3d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1d5mgs7</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>These nails look super sweet! 🍬💅</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5mgs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1d5knjw</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Such a weird nail design!</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d5knjw</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>